<commit_message>
corrected error in excel example
</commit_message>
<xml_diff>
--- a/resultsexample.xlsx
+++ b/resultsexample.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregory Liénard\Source\Repos\html-to-sql\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82816890-B3E9-4707-AFBD-BE4E7D669889}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10725" activeTab="2" xr2:uid="{AFEBECE7-5F56-41F9-B7AA-5089C81F4546}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10730"/>
   </bookViews>
   <sheets>
     <sheet name="Words" sheetId="1" r:id="rId1"/>
     <sheet name="Links" sheetId="2" r:id="rId2"/>
     <sheet name="Page" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -206,9 +200,6 @@
     <t>!</t>
   </si>
   <si>
-    <t>dfn</t>
-  </si>
-  <si>
     <t>Header1</t>
   </si>
   <si>
@@ -429,12 +420,15 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>HTML</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,7 +477,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -787,38 +781,38 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3E55B9-F667-4F20-B556-D800164F4F67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH50" sqref="AH50"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:AP16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="9" style="1"/>
-    <col min="10" max="10" width="32.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="32.26953125" style="1" customWidth="1"/>
     <col min="11" max="34" width="9" style="1"/>
-    <col min="35" max="35" width="11.42578125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="11.453125" style="1" customWidth="1"/>
     <col min="36" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -842,7 +836,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>8</v>
@@ -941,7 +935,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1030,10 +1024,10 @@
         <v>0</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF2" s="1">
         <v>1</v>
@@ -1069,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1158,10 +1152,10 @@
         <v>0</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF3" s="1">
         <v>1</v>
@@ -1197,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1286,10 +1280,10 @@
         <v>0</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF4" s="1">
         <v>1</v>
@@ -1325,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1414,10 +1408,10 @@
         <v>0</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF5" s="1">
         <v>1</v>
@@ -1453,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1542,10 +1536,10 @@
         <v>0</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF6" s="1">
         <v>1</v>
@@ -1581,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1670,10 +1664,10 @@
         <v>0</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF7" s="1">
         <v>1</v>
@@ -1709,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1798,10 +1792,10 @@
         <v>0</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF8" s="1">
         <v>1</v>
@@ -1837,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1926,10 +1920,10 @@
         <v>0</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF9" s="1">
         <v>1</v>
@@ -1965,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2054,10 +2048,10 @@
         <v>0</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF10" s="1">
         <v>1</v>
@@ -2093,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2182,10 +2176,10 @@
         <v>0</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF11" s="1">
         <v>1</v>
@@ -2221,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2310,10 +2304,10 @@
         <v>0</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF12" s="1">
         <v>1</v>
@@ -2349,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2438,10 +2432,10 @@
         <v>0</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF13" s="1">
         <v>1</v>
@@ -2477,7 +2471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2566,10 +2560,10 @@
         <v>0</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF14" s="1">
         <v>1</v>
@@ -2605,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2694,10 +2688,10 @@
         <v>0</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF15" s="1">
         <v>1</v>
@@ -2733,12 +2727,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -2822,10 +2816,10 @@
         <v>0</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE16" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF16" s="1">
         <v>1</v>
@@ -2843,7 +2837,7 @@
         <v>0</v>
       </c>
       <c r="AK16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL16" s="1">
         <v>0</v>
@@ -2861,12 +2855,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -2950,10 +2944,10 @@
         <v>0</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF17" s="1">
         <v>1</v>
@@ -2989,12 +2983,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -3078,10 +3072,10 @@
         <v>0</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF18" s="1">
         <v>1</v>
@@ -3117,12 +3111,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -3206,10 +3200,10 @@
         <v>0</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF19" s="1">
         <v>1</v>
@@ -3245,12 +3239,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -3334,10 +3328,10 @@
         <v>0</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE20" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF20" s="1">
         <v>1</v>
@@ -3373,12 +3367,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -3462,10 +3456,10 @@
         <v>0</v>
       </c>
       <c r="AD21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE21" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF21" s="1">
         <v>1</v>
@@ -3501,12 +3495,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -3590,10 +3584,10 @@
         <v>0</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF22" s="1">
         <v>1</v>
@@ -3629,7 +3623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3718,10 +3712,10 @@
         <v>0</v>
       </c>
       <c r="AD23" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF23" s="1">
         <v>1</v>
@@ -3733,7 +3727,7 @@
         <v>41</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AJ23" s="1">
         <v>0</v>
@@ -3757,12 +3751,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -3846,10 +3840,10 @@
         <v>0</v>
       </c>
       <c r="AD24" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE24" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF24" s="1">
         <v>1</v>
@@ -3885,100 +3879,100 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>0</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1">
+        <v>0</v>
+      </c>
+      <c r="U25" s="1">
+        <v>0</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0</v>
+      </c>
+      <c r="W25" s="1">
+        <v>0</v>
+      </c>
+      <c r="X25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K25" s="1">
-        <v>0</v>
-      </c>
-      <c r="L25" s="1">
-        <v>0</v>
-      </c>
-      <c r="M25" s="1">
-        <v>0</v>
-      </c>
-      <c r="N25" s="1">
-        <v>0</v>
-      </c>
-      <c r="O25" s="1">
-        <v>0</v>
-      </c>
-      <c r="P25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>0</v>
-      </c>
-      <c r="R25" s="1">
-        <v>0</v>
-      </c>
-      <c r="S25" s="1">
-        <v>0</v>
-      </c>
-      <c r="T25" s="1">
-        <v>0</v>
-      </c>
-      <c r="U25" s="1">
-        <v>0</v>
-      </c>
-      <c r="V25" s="1">
-        <v>0</v>
-      </c>
-      <c r="W25" s="1">
-        <v>0</v>
-      </c>
-      <c r="X25" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC25" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD25" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE25" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="AF25" s="1">
         <v>1</v>
       </c>
@@ -4013,12 +4007,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -4102,10 +4096,10 @@
         <v>0</v>
       </c>
       <c r="AD26" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE26" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF26" s="1">
         <v>1</v>
@@ -4141,12 +4135,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
@@ -4230,10 +4224,10 @@
         <v>0</v>
       </c>
       <c r="AD27" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE27" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF27" s="1">
         <v>1</v>
@@ -4269,12 +4263,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -4358,10 +4352,10 @@
         <v>1</v>
       </c>
       <c r="AD28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE28" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF28" s="1">
         <v>1</v>
@@ -4397,12 +4391,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -4486,10 +4480,10 @@
         <v>1</v>
       </c>
       <c r="AD29" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE29" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF29" s="1">
         <v>1</v>
@@ -4525,37 +4519,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0</v>
-      </c>
-      <c r="I30" s="1">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="K30" s="1">
         <v>0</v>
       </c>
@@ -4614,10 +4608,10 @@
         <v>0</v>
       </c>
       <c r="AD30" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE30" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF30" s="1">
         <v>1</v>
@@ -4653,12 +4647,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -4742,10 +4736,10 @@
         <v>0</v>
       </c>
       <c r="AD31" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE31" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF31" s="1">
         <v>1</v>
@@ -4781,12 +4775,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -4870,10 +4864,10 @@
         <v>0</v>
       </c>
       <c r="AD32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE32" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF32" s="1">
         <v>1</v>
@@ -4909,37 +4903,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="1">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
-      <c r="H33" s="1">
-        <v>0</v>
-      </c>
-      <c r="I33" s="1">
-        <v>1</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="K33" s="1">
         <v>1</v>
       </c>
@@ -4998,10 +4992,10 @@
         <v>0</v>
       </c>
       <c r="AD33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE33" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF33" s="1">
         <v>1</v>
@@ -5037,12 +5031,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
@@ -5126,10 +5120,10 @@
         <v>0</v>
       </c>
       <c r="AD34" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE34" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF34" s="1">
         <v>1</v>
@@ -5165,12 +5159,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
@@ -5254,10 +5248,10 @@
         <v>0</v>
       </c>
       <c r="AD35" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE35" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF35" s="1">
         <v>1</v>
@@ -5293,12 +5287,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36" s="1">
         <v>0</v>
@@ -5382,10 +5376,10 @@
         <v>0</v>
       </c>
       <c r="AD36" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE36" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF36" s="1">
         <v>1</v>
@@ -5421,12 +5415,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
@@ -5510,10 +5504,10 @@
         <v>0</v>
       </c>
       <c r="AD37" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE37" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF37" s="1">
         <v>1</v>
@@ -5549,12 +5543,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1">
         <v>0</v>
@@ -5638,23 +5632,23 @@
         <v>0</v>
       </c>
       <c r="AD38" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI38" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AF38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH38" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI38" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="AJ38" s="1">
         <v>0</v>
       </c>
@@ -5677,12 +5671,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
@@ -5706,7 +5700,7 @@
         <v>1</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K39" s="1">
         <v>0</v>
@@ -5766,10 +5760,10 @@
         <v>0</v>
       </c>
       <c r="AD39" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE39" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF39" s="1">
         <v>1</v>
@@ -5805,12 +5799,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
@@ -5834,7 +5828,7 @@
         <v>1</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K40" s="1">
         <v>0</v>
@@ -5894,10 +5888,10 @@
         <v>0</v>
       </c>
       <c r="AD40" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE40" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF40" s="1">
         <v>1</v>
@@ -5933,12 +5927,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="1">
         <v>0</v>
@@ -5962,7 +5956,7 @@
         <v>1</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K41" s="1">
         <v>0</v>
@@ -6022,10 +6016,10 @@
         <v>0</v>
       </c>
       <c r="AD41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE41" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF41" s="1">
         <v>1</v>
@@ -6061,12 +6055,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1">
         <v>0</v>
@@ -6150,10 +6144,10 @@
         <v>0</v>
       </c>
       <c r="AD42" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE42" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF42" s="1">
         <v>1</v>
@@ -6189,12 +6183,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="1">
         <v>0</v>
@@ -6278,10 +6272,10 @@
         <v>0</v>
       </c>
       <c r="AD43" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE43" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF43" s="1">
         <v>1</v>
@@ -6317,12 +6311,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" s="1">
         <v>0</v>
@@ -6406,10 +6400,10 @@
         <v>0</v>
       </c>
       <c r="AD44" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE44" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF44" s="1">
         <v>1</v>
@@ -6445,12 +6439,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" s="1">
         <v>0</v>
@@ -6534,10 +6528,10 @@
         <v>0</v>
       </c>
       <c r="AD45" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE45" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF45" s="1">
         <v>1</v>
@@ -6573,12 +6567,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" s="1">
         <v>0</v>
@@ -6662,10 +6656,10 @@
         <v>0</v>
       </c>
       <c r="AD46" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE46" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF46" s="1">
         <v>1</v>
@@ -6701,37 +6695,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0</v>
+      </c>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="1">
-        <v>0</v>
-      </c>
-      <c r="D47" s="1">
-        <v>0</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-      <c r="F47" s="1">
-        <v>0</v>
-      </c>
-      <c r="G47" s="1">
-        <v>0</v>
-      </c>
-      <c r="H47" s="1">
-        <v>0</v>
-      </c>
-      <c r="I47" s="1">
-        <v>1</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="K47" s="1">
         <v>0</v>
       </c>
@@ -6790,10 +6784,10 @@
         <v>0</v>
       </c>
       <c r="AD47" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE47" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF47" s="1">
         <v>1</v>
@@ -6829,12 +6823,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C48" s="1">
         <v>0</v>
@@ -6858,7 +6852,7 @@
         <v>1</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K48" s="1">
         <v>0</v>
@@ -6918,10 +6912,10 @@
         <v>0</v>
       </c>
       <c r="AD48" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE48" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF48" s="1">
         <v>1</v>
@@ -6957,12 +6951,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C49" s="1">
         <v>0</v>
@@ -6986,7 +6980,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K49" s="1">
         <v>0</v>
@@ -7046,10 +7040,10 @@
         <v>0</v>
       </c>
       <c r="AD49" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE49" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF49" s="1">
         <v>1</v>
@@ -7085,12 +7079,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C50" s="1">
         <v>0</v>
@@ -7174,10 +7168,10 @@
         <v>0</v>
       </c>
       <c r="AD50" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE50" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF50" s="1">
         <v>1</v>
@@ -7213,12 +7207,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
@@ -7302,10 +7296,10 @@
         <v>0</v>
       </c>
       <c r="AD51" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE51" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF51" s="1">
         <v>1</v>
@@ -7341,12 +7335,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C52" s="1">
         <v>0</v>
@@ -7430,10 +7424,10 @@
         <v>0</v>
       </c>
       <c r="AD52" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE52" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF52" s="1">
         <v>1</v>
@@ -7469,12 +7463,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
@@ -7558,10 +7552,10 @@
         <v>0</v>
       </c>
       <c r="AD53" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE53" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF53" s="1">
         <v>1</v>
@@ -7597,7 +7591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -7686,10 +7680,10 @@
         <v>0</v>
       </c>
       <c r="AD54" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE54" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF54" s="1">
         <v>1</v>
@@ -7698,7 +7692,7 @@
         <v>1</v>
       </c>
       <c r="AH54" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AI54" s="1" t="s">
         <v>41</v>
@@ -7725,12 +7719,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
@@ -7814,10 +7808,10 @@
         <v>0</v>
       </c>
       <c r="AD55" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE55" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF55" s="1">
         <v>1</v>
@@ -7853,7 +7847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -7981,12 +7975,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" s="1">
         <v>0</v>
@@ -8070,10 +8064,10 @@
         <v>0</v>
       </c>
       <c r="AD57" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE57" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF57" s="1">
         <v>1</v>
@@ -8109,12 +8103,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C58" s="1">
         <v>0</v>
@@ -8198,10 +8192,10 @@
         <v>0</v>
       </c>
       <c r="AD58" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE58" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF58" s="1">
         <v>1</v>
@@ -8237,12 +8231,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C59" s="1">
         <v>0</v>
@@ -8326,10 +8320,10 @@
         <v>0</v>
       </c>
       <c r="AD59" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE59" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF59" s="1">
         <v>1</v>
@@ -8365,12 +8359,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
@@ -8454,10 +8448,10 @@
         <v>0</v>
       </c>
       <c r="AD60" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE60" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF60" s="1">
         <v>1</v>
@@ -8493,12 +8487,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C61" s="1">
         <v>0</v>
@@ -8582,10 +8576,10 @@
         <v>0</v>
       </c>
       <c r="AD61" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE61" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF61" s="1">
         <v>1</v>
@@ -8621,37 +8615,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C62" s="1">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1">
-        <v>0</v>
-      </c>
-      <c r="E62" s="1">
-        <v>0</v>
-      </c>
-      <c r="F62" s="1">
-        <v>0</v>
-      </c>
-      <c r="G62" s="1">
-        <v>0</v>
-      </c>
-      <c r="H62" s="1">
-        <v>0</v>
-      </c>
-      <c r="I62" s="1">
-        <v>0</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="K62" s="1">
         <v>0</v>
       </c>
@@ -8710,10 +8704,10 @@
         <v>0</v>
       </c>
       <c r="AD62" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE62" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF62" s="1">
         <v>1</v>
@@ -8749,37 +8743,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="1">
-        <v>0</v>
-      </c>
-      <c r="D63" s="1">
-        <v>0</v>
-      </c>
-      <c r="E63" s="1">
-        <v>0</v>
-      </c>
-      <c r="F63" s="1">
-        <v>0</v>
-      </c>
-      <c r="G63" s="1">
-        <v>0</v>
-      </c>
-      <c r="H63" s="1">
-        <v>0</v>
-      </c>
-      <c r="I63" s="1">
-        <v>0</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="K63" s="1">
         <v>0</v>
       </c>
@@ -8838,10 +8832,10 @@
         <v>0</v>
       </c>
       <c r="AD63" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE63" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF63" s="1">
         <v>1</v>
@@ -8877,37 +8871,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="1">
-        <v>0</v>
-      </c>
-      <c r="D64" s="1">
-        <v>0</v>
-      </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-      <c r="F64" s="1">
-        <v>0</v>
-      </c>
-      <c r="G64" s="1">
-        <v>0</v>
-      </c>
-      <c r="H64" s="1">
-        <v>0</v>
-      </c>
-      <c r="I64" s="1">
-        <v>0</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="K64" s="1">
         <v>0</v>
       </c>
@@ -8966,10 +8960,10 @@
         <v>0</v>
       </c>
       <c r="AD64" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE64" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF64" s="1">
         <v>1</v>
@@ -9005,37 +8999,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="J65" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C65" s="1">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1">
-        <v>0</v>
-      </c>
-      <c r="E65" s="1">
-        <v>0</v>
-      </c>
-      <c r="F65" s="1">
-        <v>0</v>
-      </c>
-      <c r="G65" s="1">
-        <v>0</v>
-      </c>
-      <c r="H65" s="1">
-        <v>0</v>
-      </c>
-      <c r="I65" s="1">
-        <v>0</v>
-      </c>
-      <c r="J65" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="K65" s="1">
         <v>1</v>
       </c>
@@ -9094,10 +9088,10 @@
         <v>0</v>
       </c>
       <c r="AD65" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE65" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF65" s="1">
         <v>1</v>
@@ -9139,37 +9133,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C5269F-9968-4FA1-B1C5-5B5A3127C6CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="79.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
         <v>116</v>
-      </c>
-      <c r="B2" t="s">
-        <v>117</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -9177,10 +9171,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -9188,10 +9182,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
         <v>119</v>
-      </c>
-      <c r="B4" t="s">
-        <v>120</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -9199,10 +9193,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -9210,10 +9204,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -9221,10 +9215,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -9232,10 +9226,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -9243,10 +9237,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -9254,10 +9248,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -9265,10 +9259,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -9276,10 +9270,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
         <v>124</v>
-      </c>
-      <c r="B12" t="s">
-        <v>125</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -9287,10 +9281,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" t="s">
         <v>126</v>
-      </c>
-      <c r="B13" t="s">
-        <v>127</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -9303,38 +9297,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1436F3-010E-4244-9B8B-C7E23A3B4852}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>27</v>
@@ -9360,10 +9354,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>